<commit_message>
versao inicial teste de geracao de estrutura
</commit_message>
<xml_diff>
--- a/Gerador_de_Modulos/biblioteca_codificacao_modulos.xlsx
+++ b/Gerador_de_Modulos/biblioteca_codificacao_modulos.xlsx
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3097,18 +3097,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3250,18 +3250,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8352C1EE-0462-49F5-9081-48505187B96A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48CFE8AE-B59B-47D6-BF2A-167AE72AE53C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48CFE8AE-B59B-47D6-BF2A-167AE72AE53C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8352C1EE-0462-49F5-9081-48505187B96A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>